<commit_message>
export to excel ws3
</commit_message>
<xml_diff>
--- a/data/ws3header.xlsx
+++ b/data/ws3header.xlsx
@@ -242,12 +242,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -258,6 +252,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -582,7 +582,8 @@
     <col min="19" max="19" width="5.85546875" customWidth="1"/>
     <col min="20" max="20" width="6.42578125" customWidth="1"/>
     <col min="21" max="21" width="7" customWidth="1"/>
-    <col min="22" max="23" width="8.85546875" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" customWidth="1"/>
     <col min="24" max="24" width="7.42578125" customWidth="1"/>
     <col min="25" max="25" width="6.42578125" customWidth="1"/>
     <col min="26" max="26" width="7" customWidth="1"/>
@@ -596,268 +597,268 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="26.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
       <c r="V1" s="1">
         <v>3</v>
       </c>
       <c r="W1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
     </row>
     <row r="2" spans="1:34" ht="15" customHeight="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11" t="s">
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="11" t="s">
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="15"/>
     </row>
     <row r="3" spans="1:34" ht="15" customHeight="1">
-      <c r="A3" s="16"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="15"/>
+      <c r="D3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11" t="s">
+      <c r="K3" s="15"/>
+      <c r="L3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11" t="s">
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="11"/>
-      <c r="AD3" s="11"/>
-      <c r="AE3" s="11" t="s">
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="15"/>
+      <c r="AB3" s="15"/>
+      <c r="AC3" s="15"/>
+      <c r="AD3" s="15"/>
+      <c r="AE3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="AF3" s="11"/>
-      <c r="AG3" s="12" t="s">
+      <c r="AF3" s="15"/>
+      <c r="AG3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="AH3" s="11" t="s">
+      <c r="AH3" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:34" ht="15" customHeight="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12" t="s">
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11" t="s">
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11" t="s">
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11" t="s">
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="11" t="s">
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="11" t="s">
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="AD4" s="11"/>
-      <c r="AE4" s="12" t="s">
+      <c r="AD4" s="15"/>
+      <c r="AE4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="AF4" s="12" t="s">
+      <c r="AF4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="AG4" s="12"/>
-      <c r="AH4" s="11"/>
+      <c r="AG4" s="16"/>
+      <c r="AH4" s="15"/>
     </row>
     <row r="5" spans="1:34" ht="59.25" customHeight="1">
-      <c r="A5" s="16"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12" t="s">
+      <c r="O5" s="16"/>
+      <c r="P5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12" t="s">
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12" t="s">
+      <c r="S5" s="16"/>
+      <c r="T5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="U5" s="12"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
-      <c r="AB5" s="11"/>
-      <c r="AC5" s="11"/>
-      <c r="AD5" s="11"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="12"/>
-      <c r="AG5" s="12"/>
-      <c r="AH5" s="11"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="16"/>
+      <c r="AF5" s="16"/>
+      <c r="AG5" s="16"/>
+      <c r="AH5" s="15"/>
     </row>
     <row r="6" spans="1:34" ht="75" customHeight="1">
-      <c r="A6" s="16"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
       <c r="G6" s="5" t="s">
         <v>21</v>
       </c>
@@ -865,10 +866,10 @@
         <v>22</v>
       </c>
       <c r="I6" s="5"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
       <c r="N6" s="4" t="s">
         <v>23</v>
       </c>
@@ -920,10 +921,10 @@
       <c r="AD6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AE6" s="12"/>
-      <c r="AF6" s="12"/>
-      <c r="AG6" s="12"/>
-      <c r="AH6" s="11"/>
+      <c r="AE6" s="16"/>
+      <c r="AF6" s="16"/>
+      <c r="AG6" s="16"/>
+      <c r="AH6" s="15"/>
     </row>
     <row r="7" spans="1:34" ht="15.75">
       <c r="A7" s="8"/>
@@ -2226,6 +2227,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="V3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AA4:AB5"/>
+    <mergeCell ref="AC4:AD5"/>
+    <mergeCell ref="AE4:AE6"/>
+    <mergeCell ref="AF4:AF6"/>
+    <mergeCell ref="V4:X5"/>
+    <mergeCell ref="Y4:Z5"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:U3"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:U4"/>
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="X1:AA1"/>
     <mergeCell ref="AB1:AE1"/>
@@ -2242,28 +2265,6 @@
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="F4:F6"/>
     <mergeCell ref="G4:I5"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:U3"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="V3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AA4:AB5"/>
-    <mergeCell ref="AC4:AD5"/>
-    <mergeCell ref="AE4:AE6"/>
-    <mergeCell ref="AF4:AF6"/>
-    <mergeCell ref="V4:X5"/>
-    <mergeCell ref="Y4:Z5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>